<commit_message>
updates tests for rml OF 1604:9
</commit_message>
<xml_diff>
--- a/tests/fixtures/orderforms/1604.9.rml.xlsx
+++ b/tests/fixtures/orderforms/1604.9.rml.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/patrikgrenfeldt/Documents/src/cg/tests/fixtures/orderforms/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D07A66A-013F-CE4E-9707-0F6F65B4393F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6A9AFF5-9082-3A49-A22D-0887EA3CCE2C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2060" yWindow="7840" windowWidth="43200" windowHeight="20180" tabRatio="211" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5042" uniqueCount="1396">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5043" uniqueCount="1396">
   <si>
     <t>&lt;TABLE HEADER&gt;</t>
   </si>
@@ -6722,8 +6722,8 @@
   </sheetPr>
   <dimension ref="A1:Z398"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A24" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="D31" sqref="D31"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="Q15" sqref="Q15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="13.6640625" defaultRowHeight="13"/>
@@ -6978,7 +6978,7 @@
       <c r="Y8" s="6"/>
       <c r="Z8" s="6"/>
     </row>
-    <row r="9" spans="1:26" s="7" customFormat="1" ht="22" hidden="1" customHeight="1">
+    <row r="9" spans="1:26" s="7" customFormat="1" ht="22" customHeight="1">
       <c r="A9" s="170" t="s">
         <v>512</v>
       </c>
@@ -7135,7 +7135,7 @@
       <c r="Y12" s="43"/>
       <c r="Z12" s="44"/>
     </row>
-    <row r="13" spans="1:26" s="11" customFormat="1" ht="56" hidden="1" customHeight="1">
+    <row r="13" spans="1:26" s="11" customFormat="1" ht="56" customHeight="1">
       <c r="A13" s="120" t="s">
         <v>73</v>
       </c>
@@ -7267,7 +7267,9 @@
         <v>A701-A501 (ATCACGAC-TGAACCTT)</v>
       </c>
       <c r="P15" s="96"/>
-      <c r="Q15" s="95"/>
+      <c r="Q15" s="95" t="s">
+        <v>1370</v>
+      </c>
       <c r="R15" s="96"/>
       <c r="S15" s="126" t="s">
         <v>1371</v>

</xml_diff>